<commit_message>
Zmiany w tresci messagebox, dodanie przypadkow testowych do scenariusza 2
</commit_message>
<xml_diff>
--- a/testy/scenariusze_testowe.xlsx
+++ b/testy/scenariusze_testowe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studia WSB - Tester oprogramowania\App_zaliczenie\App_zaliczenie\testy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BB2ED-0E79-4889-9003-525B469A12CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7618F16-5108-41B2-B20D-0DD834E79EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="179">
   <si>
     <t>Scenariusze testowe:</t>
   </si>
@@ -377,9 +377,6 @@
     <t>Kliknięcie przycisku "Pokaż wszystkie"</t>
   </si>
   <si>
-    <t>Uruchomienie aplikacji - wyświetla się menu aplikacji</t>
-  </si>
-  <si>
     <t>W dolnej sekcji okna o nazwie "Wydatki" pojawia się tabela z danymi z bazy danych(patrz zakładke "Dane do bazy danych" i screen ponizej)</t>
   </si>
   <si>
@@ -495,6 +492,81 @@
   </si>
   <si>
     <t>W polu wybierania  o nazwie "Wybierz miesiąc" wyświetla się nazwa "styczeń"</t>
+  </si>
+  <si>
+    <t>Wyświetla się menu aplikacji</t>
+  </si>
+  <si>
+    <t>Uruchomienie aplikacji</t>
+  </si>
+  <si>
+    <t>Potwierdzenie wartości domyślnej z pola o nazwie "Wpisz rok" (domyślna wartość to: "2024")</t>
+  </si>
+  <si>
+    <t>W polu "Wpisz rok" wyświetla się wartość "2024"</t>
+  </si>
+  <si>
+    <t>Kliknięcie przycisku "Pokaż z miesiąca"</t>
+  </si>
+  <si>
+    <t>Przypadek testowy 2.8.</t>
+  </si>
+  <si>
+    <t>Użytkownikowi po wpisaniu ręcznie wartości "100" w polu wybierz miesiąc i wpisaniu roku (domyślnie 2024) oraz kliknięciu w przycisk "Pokaż z miesiąca" powinien zostać wyświetlony messagebox o treści: "Wybrano błędny miesiąc."</t>
+  </si>
+  <si>
+    <t>W polu wybierania  o nazwie "Wybierz miesiąc" wyświetla się wartość "100"</t>
+  </si>
+  <si>
+    <t>Wpisanie ręcznie w polu "Wybierz miesiąć" wartości "100"</t>
+  </si>
+  <si>
+    <t>Użytkownikowi po wpisaniu ręcznie wartości "słowo" w polu wybierz miesiąc i wpisaniu roku (domyślnie 2024) oraz kliknięciu w przycisk "Pokaż z miesiąca" powinien zostać wyświetlony messagebox o treści: "Wybrano błędny miesiąc."</t>
+  </si>
+  <si>
+    <t>Wpisanie ręcznie w polu "Wybierz miesiąć" wartości "słowo"</t>
+  </si>
+  <si>
+    <t>W polu wybierania  o nazwie "Wybierz miesiąc" wyświetla się wartość "słowo"</t>
+  </si>
+  <si>
+    <t>Wyświetlanie wydatków z danego miesiąca z bazy danych aplikacji z nie poprawnie wpisanymi danymi - w polu "Wybierz miesiąc" wpisano inne słowo niż podpowiada lista rozwijana</t>
+  </si>
+  <si>
+    <t>Wyświetlanie wydatków z danego miesiąca z bazy danych aplikacji z nie poprawnie wpisanymi danymi - w polu "Wybierz miesiąc" wpisano wartość liczbową</t>
+  </si>
+  <si>
+    <t>Wyświetlanie wydatków z danego miesiąca z bazy danych aplikacji z nie poprawnie wpisanymi danymi - w polu "Wpisz rok" wpisano niepoprawną dodatnią wartość liczbową</t>
+  </si>
+  <si>
+    <t>Wpisanie ręcznie w polu "Wpisz rok" wartości "25"</t>
+  </si>
+  <si>
+    <t>W polu "Wpisz rok" wyświetla się wartość "25"</t>
+  </si>
+  <si>
+    <t>Użytkownikowi po wybraniu miesiąca z listy rozwijanej i wpisaniu niepoprawnej liczbowej wartości "25" w polu "Wpisz rok" oraz kliknięciu w przycisk "Pokaż z miesiąca" powinien zostać wyświetlony messagebox o treści: "Wybrano niepoprawny rok!"</t>
+  </si>
+  <si>
+    <t>Wyświetlanie wydatków z danego miesiąca z bazy danych aplikacji z nie poprawnie wpisanymi danymi - w polu "Wpisz rok" wpisano niepoprawną ujemną wartość liczbową</t>
+  </si>
+  <si>
+    <t>Użytkownikowi po wybraniu miesiąca z listy rozwijanej i wpisaniu niepoprawnej wartości "-35,2" w polu "Wpisz rok" oraz kliknięciu w przycisk "Pokaż z miesiąca" powinien zostać wyświetlony messagebox o treści: "Wybrano niepoprawny rok!"</t>
+  </si>
+  <si>
+    <t>W polu "Wpisz rok" wyświetla się wartość "-35,2"</t>
+  </si>
+  <si>
+    <t>Wyświetlanie wydatków z danego miesiąca z bazy danych aplikacji z nie poprawnie wpisanymi danymi - w polu "Wpisz rok" wpisano niepoprawną  wartość ciągu znaków</t>
+  </si>
+  <si>
+    <t>Użytkownikowi po wybraniu miesiąca z listy rozwijanej i wpisaniu niepoprawnej  wartości (ciąg znaków) "rok" w polu "Wpisz rok" oraz kliknięciu w przycisk "Pokaż z miesiąca" powinien zostać wyświetlony messagebox o treści: "Wybrano niepoprawny rok!"</t>
+  </si>
+  <si>
+    <t>Wpisanie ręcznie w polu "Wpisz rok" wartości "rok"</t>
+  </si>
+  <si>
+    <t>W polu "Wpisz rok" wyświetla się wartość "rok"</t>
   </si>
 </sst>
 </file>
@@ -699,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -768,6 +840,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -777,7 +855,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -792,35 +876,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,8 +926,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBCEFEE"/>
       <color rgb="FFDFE6E7"/>
-      <color rgb="FFBCEFEE"/>
       <color rgb="FFD1F4F3"/>
       <color rgb="FF33CCCC"/>
       <color rgb="FF00FFFF"/>
@@ -1585,6 +1681,255 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5570282</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Obraz 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C4AFF8-0791-6350-BEE5-861C58339ADF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8953500" y="75952350"/>
+          <a:ext cx="5427407" cy="2438400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1876426</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>253998</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3800476</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>1533715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Obraz 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AD2CCED-0932-B352-A58B-85D5BC470A26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10687051" y="80416398"/>
+          <a:ext cx="1924050" cy="1279717"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1876426</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>253998</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1924050" cy="1279717"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Obraz 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4B48D87-BA44-49A5-8E64-368388D2CD32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10687051" y="80416398"/>
+          <a:ext cx="1924050" cy="1279717"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1800225</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>241631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3895725</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>1571818</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Obraz 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C731B5D-47EF-38BA-2250-AA823BCD9838}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10610850" y="87814481"/>
+          <a:ext cx="2095500" cy="1330187"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1800225</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>241631</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2095500" cy="1330187"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Obraz 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{350FA03F-3C77-44E7-B0B7-D3CF34216C02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10610850" y="87814481"/>
+          <a:ext cx="2095500" cy="1330187"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1800225</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>241631</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2095500" cy="1330187"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Obraz 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6BCF5C2-022F-497A-8A13-FE1410EE4D25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10610850" y="87814481"/>
+          <a:ext cx="2095500" cy="1330187"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1854,7 +2199,7 @@
   <dimension ref="B1:F315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,10 +2219,10 @@
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="2:6" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3288,11 +3633,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0953F3B-78FC-43F3-9402-DE0C5199EBA3}">
-  <dimension ref="A1:J497"/>
+  <dimension ref="A1:J496"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F129" sqref="F129"/>
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H156" sqref="H156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,36 +3687,38 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="30">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="34">
         <v>1</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="34">
         <v>1</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" s="13"/>
+        <v>155</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>154</v>
+      </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="9" t="s">
         <v>19</v>
       </c>
@@ -3385,11 +3732,11 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="9" t="s">
         <v>23</v>
       </c>
@@ -3403,11 +3750,11 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="9" t="s">
         <v>26</v>
       </c>
@@ -3421,11 +3768,11 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="9" t="s">
         <v>29</v>
       </c>
@@ -3439,11 +3786,11 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="9" t="s">
         <v>32</v>
       </c>
@@ -3457,11 +3804,11 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="9" t="s">
         <v>35</v>
       </c>
@@ -3475,11 +3822,11 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
       <c r="F9" s="9" t="s">
         <v>37</v>
       </c>
@@ -3492,36 +3839,38 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="27">
         <v>1</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="27">
         <v>2</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="27" t="s">
         <v>68</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" s="11"/>
+        <v>155</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>154</v>
+      </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
     </row>
-    <row r="11" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
       <c r="F11" s="11" t="s">
         <v>19</v>
       </c>
@@ -3535,11 +3884,11 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
       <c r="F12" s="11" t="s">
         <v>23</v>
       </c>
@@ -3553,11 +3902,11 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
       <c r="F13" s="11" t="s">
         <v>26</v>
       </c>
@@ -3571,11 +3920,11 @@
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="11" t="s">
         <v>29</v>
       </c>
@@ -3589,11 +3938,11 @@
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="11" t="s">
         <v>32</v>
       </c>
@@ -3607,11 +3956,11 @@
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
       <c r="F16" s="11" t="s">
         <v>35</v>
       </c>
@@ -3625,11 +3974,11 @@
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
       <c r="F17" s="11" t="s">
         <v>37</v>
       </c>
@@ -3643,11 +3992,11 @@
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
       <c r="F18" s="11" t="s">
         <v>47</v>
       </c>
@@ -3660,36 +4009,38 @@
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="26">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="30"/>
+      <c r="B19" s="28">
         <v>1</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="28">
         <v>3</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="28" t="s">
         <v>69</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H19" s="9"/>
+        <v>155</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
       <c r="F20" s="9" t="s">
         <v>19</v>
       </c>
@@ -3703,11 +4054,11 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
       <c r="F21" s="9" t="s">
         <v>23</v>
       </c>
@@ -3721,11 +4072,11 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="9" t="s">
         <v>26</v>
       </c>
@@ -3739,11 +4090,11 @@
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
       <c r="F23" s="9" t="s">
         <v>29</v>
       </c>
@@ -3757,11 +4108,11 @@
       <c r="J23" s="9"/>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
       <c r="F24" s="9" t="s">
         <v>32</v>
       </c>
@@ -3775,11 +4126,11 @@
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="1:10" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
       <c r="F25" s="9" t="s">
         <v>35</v>
       </c>
@@ -3793,11 +4144,11 @@
       <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
       <c r="F26" s="9" t="s">
         <v>37</v>
       </c>
@@ -3811,11 +4162,11 @@
       <c r="J26" s="9"/>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
       <c r="F27" s="9" t="s">
         <v>47</v>
       </c>
@@ -3828,36 +4179,38 @@
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="27">
         <v>1</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="27">
         <v>4</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="27" t="s">
         <v>69</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" s="11"/>
+        <v>155</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>154</v>
+      </c>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
       <c r="F29" s="11" t="s">
         <v>19</v>
       </c>
@@ -3871,11 +4224,11 @@
       <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
       <c r="F30" s="11" t="s">
         <v>23</v>
       </c>
@@ -3889,11 +4242,11 @@
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
       <c r="F31" s="11" t="s">
         <v>26</v>
       </c>
@@ -3907,11 +4260,11 @@
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
       <c r="F32" s="11" t="s">
         <v>29</v>
       </c>
@@ -3925,11 +4278,11 @@
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
       <c r="F33" s="11" t="s">
         <v>32</v>
       </c>
@@ -3943,11 +4296,11 @@
       <c r="J33" s="11"/>
     </row>
     <row r="34" spans="1:10" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
       <c r="F34" s="11" t="s">
         <v>35</v>
       </c>
@@ -3961,11 +4314,11 @@
       <c r="J34" s="11"/>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
       <c r="F35" s="11" t="s">
         <v>37</v>
       </c>
@@ -3979,11 +4332,11 @@
       <c r="J35" s="11"/>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
       <c r="F36" s="11" t="s">
         <v>47</v>
       </c>
@@ -3996,36 +4349,38 @@
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
     </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
-      <c r="B37" s="26">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="30"/>
+      <c r="B37" s="28">
         <v>1</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="28">
         <v>5</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E37" s="28" t="s">
         <v>66</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H37" s="9"/>
+        <v>155</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
       <c r="F38" s="9" t="s">
         <v>19</v>
       </c>
@@ -4039,11 +4394,11 @@
       <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
       <c r="F39" s="9" t="s">
         <v>23</v>
       </c>
@@ -4057,11 +4412,11 @@
       <c r="J39" s="9"/>
     </row>
     <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
       <c r="F40" s="9" t="s">
         <v>26</v>
       </c>
@@ -4075,11 +4430,11 @@
       <c r="J40" s="9"/>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
       <c r="F41" s="9" t="s">
         <v>29</v>
       </c>
@@ -4093,11 +4448,11 @@
       <c r="J41" s="9"/>
     </row>
     <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
       <c r="F42" s="9" t="s">
         <v>32</v>
       </c>
@@ -4111,11 +4466,11 @@
       <c r="J42" s="9"/>
     </row>
     <row r="43" spans="1:10" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="36"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
       <c r="F43" s="9" t="s">
         <v>35</v>
       </c>
@@ -4129,11 +4484,11 @@
       <c r="J43" s="9"/>
     </row>
     <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
       <c r="F44" s="9" t="s">
         <v>37</v>
       </c>
@@ -4147,11 +4502,11 @@
       <c r="J44" s="9"/>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
       <c r="F45" s="9" t="s">
         <v>47</v>
       </c>
@@ -4164,36 +4519,38 @@
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
     </row>
-    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
-      <c r="B46" s="25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="30"/>
+      <c r="B46" s="27">
         <v>1</v>
       </c>
-      <c r="C46" s="25">
+      <c r="C46" s="27">
         <v>6</v>
       </c>
-      <c r="D46" s="25" t="s">
+      <c r="D46" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="25" t="s">
+      <c r="E46" s="27" t="s">
         <v>79</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H46" s="11"/>
+        <v>155</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>154</v>
+      </c>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="36"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
       <c r="F47" s="11" t="s">
         <v>19</v>
       </c>
@@ -4207,11 +4564,11 @@
       <c r="J47" s="11"/>
     </row>
     <row r="48" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="36"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
       <c r="F48" s="11" t="s">
         <v>23</v>
       </c>
@@ -4225,11 +4582,11 @@
       <c r="J48" s="11"/>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
       <c r="F49" s="11" t="s">
         <v>26</v>
       </c>
@@ -4243,11 +4600,11 @@
       <c r="J49" s="11"/>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="36"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
       <c r="F50" s="11" t="s">
         <v>29</v>
       </c>
@@ -4261,11 +4618,11 @@
       <c r="J50" s="11"/>
     </row>
     <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
       <c r="F51" s="11" t="s">
         <v>32</v>
       </c>
@@ -4279,11 +4636,11 @@
       <c r="J51" s="11"/>
     </row>
     <row r="52" spans="1:10" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="36"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
       <c r="F52" s="11" t="s">
         <v>35</v>
       </c>
@@ -4297,11 +4654,11 @@
       <c r="J52" s="11"/>
     </row>
     <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="36"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
       <c r="F53" s="11" t="s">
         <v>37</v>
       </c>
@@ -4315,11 +4672,11 @@
       <c r="J53" s="11"/>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="36"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
       <c r="F54" s="11" t="s">
         <v>47</v>
       </c>
@@ -4332,36 +4689,38 @@
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
     </row>
-    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="36"/>
-      <c r="B55" s="26">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="30"/>
+      <c r="B55" s="28">
         <v>1</v>
       </c>
-      <c r="C55" s="26">
+      <c r="C55" s="28">
         <v>7</v>
       </c>
-      <c r="D55" s="26" t="s">
+      <c r="D55" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="26" t="s">
+      <c r="E55" s="28" t="s">
         <v>76</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H55" s="9"/>
+        <v>155</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="36"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
       <c r="F56" s="9" t="s">
         <v>19</v>
       </c>
@@ -4375,11 +4734,11 @@
       <c r="J56" s="9"/>
     </row>
     <row r="57" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="36"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
       <c r="F57" s="9" t="s">
         <v>23</v>
       </c>
@@ -4393,11 +4752,11 @@
       <c r="J57" s="9"/>
     </row>
     <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="36"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
       <c r="F58" s="9" t="s">
         <v>26</v>
       </c>
@@ -4411,11 +4770,11 @@
       <c r="J58" s="9"/>
     </row>
     <row r="59" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="36"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
       <c r="F59" s="9" t="s">
         <v>29</v>
       </c>
@@ -4429,11 +4788,11 @@
       <c r="J59" s="9"/>
     </row>
     <row r="60" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="36"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
       <c r="F60" s="9" t="s">
         <v>32</v>
       </c>
@@ -4447,11 +4806,11 @@
       <c r="J60" s="9"/>
     </row>
     <row r="61" spans="1:10" ht="132" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="36"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
       <c r="F61" s="9" t="s">
         <v>35</v>
       </c>
@@ -4465,11 +4824,11 @@
       <c r="J61" s="9"/>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="36"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
       <c r="F62" s="9" t="s">
         <v>37</v>
       </c>
@@ -4482,36 +4841,38 @@
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
     </row>
-    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="36"/>
-      <c r="B63" s="25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="30"/>
+      <c r="B63" s="27">
         <v>1</v>
       </c>
-      <c r="C63" s="25">
+      <c r="C63" s="27">
         <v>8</v>
       </c>
-      <c r="D63" s="25" t="s">
+      <c r="D63" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="E63" s="25" t="s">
+      <c r="E63" s="27" t="s">
         <v>81</v>
       </c>
       <c r="F63" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H63" s="11"/>
+        <v>155</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>154</v>
+      </c>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="36"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
+      <c r="A64" s="30"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
       <c r="F64" s="11" t="s">
         <v>19</v>
       </c>
@@ -4525,11 +4886,11 @@
       <c r="J64" s="11"/>
     </row>
     <row r="65" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="36"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
       <c r="F65" s="11" t="s">
         <v>23</v>
       </c>
@@ -4543,11 +4904,11 @@
       <c r="J65" s="11"/>
     </row>
     <row r="66" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="36"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
+      <c r="A66" s="30"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
       <c r="F66" s="11" t="s">
         <v>26</v>
       </c>
@@ -4561,11 +4922,11 @@
       <c r="J66" s="11"/>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="36"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="27"/>
       <c r="F67" s="11" t="s">
         <v>29</v>
       </c>
@@ -4579,11 +4940,11 @@
       <c r="J67" s="11"/>
     </row>
     <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="36"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27"/>
       <c r="F68" s="11" t="s">
         <v>32</v>
       </c>
@@ -4597,11 +4958,11 @@
       <c r="J68" s="11"/>
     </row>
     <row r="69" spans="1:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="36"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
       <c r="F69" s="11" t="s">
         <v>35</v>
       </c>
@@ -4615,11 +4976,11 @@
       <c r="J69" s="11"/>
     </row>
     <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="36"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
+      <c r="A70" s="30"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="27"/>
       <c r="F70" s="11" t="s">
         <v>37</v>
       </c>
@@ -4633,11 +4994,11 @@
       <c r="J70" s="11"/>
     </row>
     <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="36"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="27"/>
       <c r="F71" s="11" t="s">
         <v>47</v>
       </c>
@@ -4650,36 +5011,38 @@
       <c r="I71" s="11"/>
       <c r="J71" s="11"/>
     </row>
-    <row r="72" spans="1:10" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="36"/>
-      <c r="B72" s="26">
+    <row r="72" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="30"/>
+      <c r="B72" s="28">
         <v>1</v>
       </c>
-      <c r="C72" s="26">
+      <c r="C72" s="28">
         <v>9</v>
       </c>
-      <c r="D72" s="26" t="s">
+      <c r="D72" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E72" s="26" t="s">
+      <c r="E72" s="28" t="s">
         <v>87</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H72" s="9"/>
+        <v>155</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>154</v>
+      </c>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
     </row>
     <row r="73" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="36"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
-      <c r="E73" s="26"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
       <c r="F73" s="9" t="s">
         <v>19</v>
       </c>
@@ -4693,11 +5056,11 @@
       <c r="J73" s="9"/>
     </row>
     <row r="74" spans="1:10" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="36"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
+      <c r="A74" s="30"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
       <c r="F74" s="9" t="s">
         <v>23</v>
       </c>
@@ -4711,11 +5074,11 @@
       <c r="J74" s="9"/>
     </row>
     <row r="75" spans="1:10" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="36"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="26"/>
+      <c r="A75" s="30"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
       <c r="F75" s="9" t="s">
         <v>26</v>
       </c>
@@ -4729,11 +5092,11 @@
       <c r="J75" s="9"/>
     </row>
     <row r="76" spans="1:10" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="36"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
-      <c r="E76" s="26"/>
+      <c r="A76" s="30"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="28"/>
       <c r="F76" s="9" t="s">
         <v>29</v>
       </c>
@@ -4747,11 +5110,11 @@
       <c r="J76" s="9"/>
     </row>
     <row r="77" spans="1:10" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="36"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
-      <c r="E77" s="26"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
       <c r="F77" s="9" t="s">
         <v>32</v>
       </c>
@@ -4765,11 +5128,11 @@
       <c r="J77" s="9"/>
     </row>
     <row r="78" spans="1:10" s="15" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="36"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="26"/>
-      <c r="D78" s="26"/>
-      <c r="E78" s="26"/>
+      <c r="A78" s="30"/>
+      <c r="B78" s="28"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
       <c r="F78" s="9" t="s">
         <v>35</v>
       </c>
@@ -4783,11 +5146,11 @@
       <c r="J78" s="9"/>
     </row>
     <row r="79" spans="1:10" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="36"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="26"/>
-      <c r="E79" s="26"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="28"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
       <c r="F79" s="9" t="s">
         <v>37</v>
       </c>
@@ -4801,11 +5164,11 @@
       <c r="J79" s="9"/>
     </row>
     <row r="80" spans="1:10" s="21" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="37"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
+      <c r="A80" s="31"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="36"/>
       <c r="F80" s="16" t="s">
         <v>47</v>
       </c>
@@ -4818,34 +5181,36 @@
       <c r="I80" s="16"/>
       <c r="J80" s="16"/>
     </row>
-    <row r="81" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="28">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="32">
         <v>2</v>
       </c>
-      <c r="C81" s="28">
+      <c r="C81" s="32">
         <v>1</v>
       </c>
-      <c r="D81" s="28" t="s">
+      <c r="D81" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E81" s="28" t="s">
+      <c r="E81" s="32" t="s">
         <v>111</v>
       </c>
       <c r="F81" s="20" t="s">
         <v>20</v>
       </c>
       <c r="G81" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H81" s="20"/>
+        <v>155</v>
+      </c>
+      <c r="H81" s="20" t="s">
+        <v>154</v>
+      </c>
       <c r="I81" s="20"/>
       <c r="J81" s="20"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
+      <c r="E82" s="27"/>
       <c r="F82" s="11" t="s">
         <v>19</v>
       </c>
@@ -4859,10 +5224,10 @@
       <c r="J82" s="11"/>
     </row>
     <row r="83" spans="2:10" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="27"/>
       <c r="F83" s="11" t="s">
         <v>23</v>
       </c>
@@ -4870,16 +5235,16 @@
         <v>114</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I83" s="11"/>
       <c r="J83" s="11"/>
     </row>
     <row r="84" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="29"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="33"/>
       <c r="F84" s="11" t="s">
         <v>26</v>
       </c>
@@ -4887,39 +5252,41 @@
         <v>49</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I84" s="11"/>
       <c r="J84" s="11"/>
     </row>
-    <row r="85" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B85" s="26">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B85" s="28">
         <v>2</v>
       </c>
-      <c r="C85" s="26">
+      <c r="C85" s="28">
         <v>2</v>
       </c>
-      <c r="D85" s="26" t="s">
+      <c r="D85" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E85" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="E85" s="26" t="s">
-        <v>126</v>
       </c>
       <c r="F85" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="H85" s="13"/>
+        <v>155</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>154</v>
+      </c>
       <c r="I85" s="13"/>
       <c r="J85" s="13"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B86" s="26"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26"/>
-      <c r="E86" s="26"/>
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="28"/>
       <c r="F86" s="9" t="s">
         <v>19</v>
       </c>
@@ -4933,61 +5300,61 @@
       <c r="J86" s="9"/>
     </row>
     <row r="87" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B87" s="26"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
+      <c r="B87" s="28"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="28"/>
       <c r="F87" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G87" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H87" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="H87" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
     </row>
     <row r="88" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B88" s="26"/>
-      <c r="C88" s="26"/>
-      <c r="D88" s="26"/>
-      <c r="E88" s="26"/>
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
       <c r="F88" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H88" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
     </row>
     <row r="89" spans="2:10" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="26"/>
-      <c r="C89" s="26"/>
-      <c r="D89" s="26"/>
-      <c r="E89" s="26"/>
+      <c r="B89" s="28"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
       <c r="F89" s="9" t="s">
         <v>29</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H89" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
     </row>
     <row r="90" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B90" s="26"/>
-      <c r="C90" s="26"/>
-      <c r="D90" s="26"/>
-      <c r="E90" s="26"/>
+      <c r="B90" s="28"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
       <c r="F90" s="9" t="s">
         <v>32</v>
       </c>
@@ -4995,789 +5362,1385 @@
         <v>49</v>
       </c>
       <c r="H90" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
     </row>
-    <row r="91" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B91" s="26">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B91" s="27">
         <v>2</v>
       </c>
-      <c r="C91" s="26">
+      <c r="C91" s="27">
         <v>3</v>
       </c>
-      <c r="D91" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="E91" s="26" t="s">
+      <c r="D91" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E91" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="F91" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G91" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="H91" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="I91" s="20"/>
+      <c r="J91" s="20"/>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B92" s="27"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H92" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+    </row>
+    <row r="93" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B93" s="27"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H93" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I93" s="11"/>
+      <c r="J93" s="11"/>
+    </row>
+    <row r="94" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B94" s="27"/>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H94" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="F91" s="13" t="s">
+      <c r="I94" s="11"/>
+      <c r="J94" s="11"/>
+    </row>
+    <row r="95" spans="2:10" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="27"/>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H95" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I95" s="11"/>
+      <c r="J95" s="11"/>
+    </row>
+    <row r="96" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B96" s="27"/>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H96" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I96" s="11"/>
+      <c r="J96" s="11"/>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B97" s="28">
+        <v>2</v>
+      </c>
+      <c r="C97" s="28">
+        <v>4</v>
+      </c>
+      <c r="D97" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F97" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G91" s="13" t="s">
+      <c r="G97" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="I97" s="13"/>
+      <c r="J97" s="13"/>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B98" s="28"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H98" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+    </row>
+    <row r="99" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B99" s="28"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G99" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="H99" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="I99" s="9"/>
+      <c r="J99" s="9"/>
+    </row>
+    <row r="100" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B100" s="28"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G100" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H100" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I100" s="9"/>
+      <c r="J100" s="9"/>
+    </row>
+    <row r="101" spans="2:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="28"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G101" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="H101" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="I101" s="9"/>
+      <c r="J101" s="9"/>
+    </row>
+    <row r="102" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B102" s="28"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G102" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H102" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="I102" s="9"/>
+      <c r="J102" s="9"/>
+    </row>
+    <row r="103" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B103" s="28"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G103" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H103" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B104" s="27">
+        <v>2</v>
+      </c>
+      <c r="C104" s="27">
+        <v>5</v>
+      </c>
+      <c r="D104" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="E104" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F104" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G104" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="H104" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="I104" s="20"/>
+      <c r="J104" s="20"/>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B105" s="27"/>
+      <c r="C105" s="27"/>
+      <c r="D105" s="27"/>
+      <c r="E105" s="27"/>
+      <c r="F105" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G105" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H105" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I105" s="11"/>
+      <c r="J105" s="11"/>
+    </row>
+    <row r="106" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B106" s="27"/>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G106" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H106" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="I106" s="11"/>
+      <c r="J106" s="11"/>
+    </row>
+    <row r="107" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B107" s="27"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G107" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="H107" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="I107" s="11"/>
+      <c r="J107" s="11"/>
+    </row>
+    <row r="108" spans="2:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="27"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G108" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H108" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I108" s="11"/>
+      <c r="J108" s="11"/>
+    </row>
+    <row r="109" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B109" s="27"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G109" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H109" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="I109" s="11"/>
+      <c r="J109" s="11"/>
+    </row>
+    <row r="110" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B110" s="27"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
+      <c r="F110" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G110" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H110" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I110" s="11"/>
+      <c r="J110" s="11"/>
+    </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B111" s="28">
+        <v>2</v>
+      </c>
+      <c r="C111" s="28">
+        <v>6</v>
+      </c>
+      <c r="D111" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E111" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F111" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G111" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="H111" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="I111" s="13"/>
+      <c r="J111" s="13"/>
+    </row>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B112" s="28"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="28"/>
+      <c r="F112" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G112" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H112" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I112" s="9"/>
+      <c r="J112" s="9"/>
+    </row>
+    <row r="113" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B113" s="28"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="28"/>
+      <c r="F113" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G113" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H113" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="I113" s="9"/>
+      <c r="J113" s="9"/>
+    </row>
+    <row r="114" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B114" s="28"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="28"/>
+      <c r="F114" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G114" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="H114" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="I114" s="9"/>
+      <c r="J114" s="9"/>
+    </row>
+    <row r="115" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="28"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="28"/>
+      <c r="E115" s="28"/>
+      <c r="F115" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G115" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="H115" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="I115" s="9"/>
+      <c r="J115" s="9"/>
+    </row>
+    <row r="116" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B116" s="28"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="28"/>
+      <c r="F116" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G116" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H116" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="I116" s="9"/>
+      <c r="J116" s="9"/>
+    </row>
+    <row r="117" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B117" s="28"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="28"/>
+      <c r="F117" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G117" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H117" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I117" s="9"/>
+      <c r="J117" s="9"/>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B118" s="27">
+        <v>2</v>
+      </c>
+      <c r="C118" s="27">
+        <v>7</v>
+      </c>
+      <c r="D118" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E118" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F118" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G118" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="H118" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="I118" s="20"/>
+      <c r="J118" s="20"/>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B119" s="27"/>
+      <c r="C119" s="27"/>
+      <c r="D119" s="27"/>
+      <c r="E119" s="27"/>
+      <c r="F119" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G119" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H119" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I119" s="11"/>
+      <c r="J119" s="11"/>
+    </row>
+    <row r="120" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B120" s="27"/>
+      <c r="C120" s="27"/>
+      <c r="D120" s="27"/>
+      <c r="E120" s="27"/>
+      <c r="F120" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G120" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H120" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="I120" s="11"/>
+      <c r="J120" s="11"/>
+    </row>
+    <row r="121" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B121" s="27"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G121" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="H121" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="I121" s="11"/>
+      <c r="J121" s="11"/>
+    </row>
+    <row r="122" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="27"/>
+      <c r="C122" s="27"/>
+      <c r="D122" s="27"/>
+      <c r="E122" s="27"/>
+      <c r="F122" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G122" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H122" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I122" s="11"/>
+      <c r="J122" s="11"/>
+    </row>
+    <row r="123" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B123" s="27"/>
+      <c r="C123" s="27"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="27"/>
+      <c r="F123" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G123" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H123" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="I123" s="11"/>
+      <c r="J123" s="11"/>
+    </row>
+    <row r="124" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B124" s="27"/>
+      <c r="C124" s="27"/>
+      <c r="D124" s="27"/>
+      <c r="E124" s="27"/>
+      <c r="F124" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G124" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H124" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I124" s="11"/>
+      <c r="J124" s="11"/>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B125" s="28">
+        <v>2</v>
+      </c>
+      <c r="C125" s="28">
+        <v>8</v>
+      </c>
+      <c r="D125" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="E125" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="F125" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="G125" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="H125" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="I125" s="13"/>
+      <c r="J125" s="13"/>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B126" s="28"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="28"/>
+      <c r="E126" s="41"/>
+      <c r="F126" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="G126" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="H126" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="I126" s="9"/>
+      <c r="J126" s="9"/>
+    </row>
+    <row r="127" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B127" s="28"/>
+      <c r="C127" s="28"/>
+      <c r="D127" s="28"/>
+      <c r="E127" s="41"/>
+      <c r="F127" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G127" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="H127" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="I127" s="9"/>
+      <c r="J127" s="9"/>
+    </row>
+    <row r="128" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B128" s="28"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="28"/>
+      <c r="E128" s="41"/>
+      <c r="F128" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="G128" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="H128" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="I128" s="9"/>
+      <c r="J128" s="9"/>
+    </row>
+    <row r="129" spans="2:10" ht="229.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="28"/>
+      <c r="C129" s="28"/>
+      <c r="D129" s="28"/>
+      <c r="E129" s="41"/>
+      <c r="F129" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G129" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="H129" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B92" s="26"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="26"/>
-      <c r="E92" s="26"/>
-      <c r="F92" s="9" t="s">
+      <c r="I129" s="9"/>
+      <c r="J129" s="9"/>
+    </row>
+    <row r="130" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B130" s="28"/>
+      <c r="C130" s="28"/>
+      <c r="D130" s="28"/>
+      <c r="E130" s="41"/>
+      <c r="F130" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="G130" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="H130" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="I130" s="9"/>
+      <c r="J130" s="9"/>
+    </row>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B131" s="27">
+        <v>2</v>
+      </c>
+      <c r="C131" s="27">
+        <v>9</v>
+      </c>
+      <c r="D131" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E131" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="F131" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G131" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="H131" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="I131" s="20"/>
+      <c r="J131" s="20"/>
+    </row>
+    <row r="132" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B132" s="27"/>
+      <c r="C132" s="27"/>
+      <c r="D132" s="27"/>
+      <c r="E132" s="45"/>
+      <c r="F132" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G92" s="9" t="s">
+      <c r="G132" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="H92" s="9" t="s">
+      <c r="H132" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="I92" s="9"/>
-      <c r="J92" s="9"/>
-    </row>
-    <row r="93" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B93" s="26"/>
-      <c r="C93" s="26"/>
-      <c r="D93" s="26"/>
-      <c r="E93" s="26"/>
-      <c r="F93" s="9" t="s">
+      <c r="I132" s="11"/>
+      <c r="J132" s="11"/>
+    </row>
+    <row r="133" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B133" s="27"/>
+      <c r="C133" s="27"/>
+      <c r="D133" s="27"/>
+      <c r="E133" s="45"/>
+      <c r="F133" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G93" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H93" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I93" s="9"/>
-      <c r="J93" s="9"/>
-    </row>
-    <row r="94" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B94" s="26"/>
-      <c r="C94" s="26"/>
-      <c r="D94" s="26"/>
-      <c r="E94" s="26"/>
-      <c r="F94" s="9" t="s">
+      <c r="G133" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="H133" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="I133" s="11"/>
+      <c r="J133" s="11"/>
+    </row>
+    <row r="134" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B134" s="27"/>
+      <c r="C134" s="27"/>
+      <c r="D134" s="27"/>
+      <c r="E134" s="45"/>
+      <c r="F134" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G94" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="H94" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="I94" s="9"/>
-      <c r="J94" s="9"/>
-    </row>
-    <row r="95" spans="2:10" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="26"/>
-      <c r="F95" s="9" t="s">
+      <c r="G134" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="H134" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="I134" s="11"/>
+      <c r="J134" s="11"/>
+    </row>
+    <row r="135" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="27"/>
+      <c r="C135" s="27"/>
+      <c r="D135" s="27"/>
+      <c r="E135" s="45"/>
+      <c r="F135" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G95" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="H95" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="I95" s="9"/>
-      <c r="J95" s="9"/>
-    </row>
-    <row r="96" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B96" s="26"/>
-      <c r="C96" s="26"/>
-      <c r="D96" s="26"/>
-      <c r="E96" s="26"/>
-      <c r="F96" s="9" t="s">
+      <c r="G135" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H135" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I135" s="11"/>
+      <c r="J135" s="11"/>
+    </row>
+    <row r="136" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B136" s="27"/>
+      <c r="C136" s="27"/>
+      <c r="D136" s="27"/>
+      <c r="E136" s="45"/>
+      <c r="F136" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="G96" s="9" t="s">
+      <c r="G136" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H136" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="I136" s="11"/>
+      <c r="J136" s="11"/>
+    </row>
+    <row r="137" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B137" s="27"/>
+      <c r="C137" s="27"/>
+      <c r="D137" s="27"/>
+      <c r="E137" s="45"/>
+      <c r="F137" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G137" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="H96" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="I96" s="9"/>
-      <c r="J96" s="9"/>
-    </row>
-    <row r="97" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B97" s="25">
+      <c r="H137" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I137" s="11"/>
+      <c r="J137" s="11"/>
+    </row>
+    <row r="138" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B138" s="28">
         <v>2</v>
       </c>
-      <c r="C97" s="25">
-        <v>4</v>
-      </c>
-      <c r="D97" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="E97" s="25" t="s">
+      <c r="C138" s="28">
+        <v>10</v>
+      </c>
+      <c r="D138" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E138" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="F138" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="G138" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="H138" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="I138" s="13"/>
+      <c r="J138" s="13"/>
+    </row>
+    <row r="139" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B139" s="28"/>
+      <c r="C139" s="28"/>
+      <c r="D139" s="28"/>
+      <c r="E139" s="47"/>
+      <c r="F139" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G139" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H139" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I139" s="9"/>
+      <c r="J139" s="9"/>
+    </row>
+    <row r="140" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B140" s="28"/>
+      <c r="C140" s="28"/>
+      <c r="D140" s="28"/>
+      <c r="E140" s="47"/>
+      <c r="F140" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G140" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="H140" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="I140" s="9"/>
+      <c r="J140" s="9"/>
+    </row>
+    <row r="141" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B141" s="28"/>
+      <c r="C141" s="28"/>
+      <c r="D141" s="28"/>
+      <c r="E141" s="47"/>
+      <c r="F141" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G141" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H141" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="I141" s="9"/>
+      <c r="J141" s="9"/>
+    </row>
+    <row r="142" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="28"/>
+      <c r="C142" s="28"/>
+      <c r="D142" s="28"/>
+      <c r="E142" s="47"/>
+      <c r="F142" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G142" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="H142" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="I142" s="9"/>
+      <c r="J142" s="9"/>
+    </row>
+    <row r="143" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B143" s="28"/>
+      <c r="C143" s="28"/>
+      <c r="D143" s="28"/>
+      <c r="E143" s="47"/>
+      <c r="F143" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G143" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H143" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="F97" s="20" t="s">
+      <c r="I143" s="9"/>
+      <c r="J143" s="9"/>
+    </row>
+    <row r="144" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B144" s="28"/>
+      <c r="C144" s="28"/>
+      <c r="D144" s="28"/>
+      <c r="E144" s="47"/>
+      <c r="F144" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G144" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H144" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I144" s="9"/>
+      <c r="J144" s="9"/>
+    </row>
+    <row r="145" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B145" s="27">
+        <v>2</v>
+      </c>
+      <c r="C145" s="27">
+        <v>11</v>
+      </c>
+      <c r="D145" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E145" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="F145" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G97" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H97" s="20"/>
-      <c r="I97" s="20"/>
-      <c r="J97" s="20"/>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B98" s="25"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="11" t="s">
+      <c r="G145" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="H145" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="I145" s="20"/>
+      <c r="J145" s="20"/>
+    </row>
+    <row r="146" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B146" s="27"/>
+      <c r="C146" s="27"/>
+      <c r="D146" s="38"/>
+      <c r="E146" s="38"/>
+      <c r="F146" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="G98" s="11" t="s">
+      <c r="G146" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="H98" s="11" t="s">
+      <c r="H146" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-    </row>
-    <row r="99" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B99" s="25"/>
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
-      <c r="F99" s="22" t="s">
+      <c r="I146" s="11"/>
+      <c r="J146" s="11"/>
+    </row>
+    <row r="147" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B147" s="27"/>
+      <c r="C147" s="27"/>
+      <c r="D147" s="38"/>
+      <c r="E147" s="38"/>
+      <c r="F147" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G99" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="H99" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="I99" s="11"/>
-      <c r="J99" s="11"/>
-    </row>
-    <row r="100" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="22" t="s">
+      <c r="G147" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H147" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="I147" s="11"/>
+      <c r="J147" s="11"/>
+    </row>
+    <row r="148" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B148" s="27"/>
+      <c r="C148" s="27"/>
+      <c r="D148" s="38"/>
+      <c r="E148" s="38"/>
+      <c r="F148" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="G100" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="H100" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
-    </row>
-    <row r="101" spans="2:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="25"/>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="22" t="s">
+      <c r="G148" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="H148" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="I148" s="11"/>
+      <c r="J148" s="11"/>
+    </row>
+    <row r="149" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="27"/>
+      <c r="C149" s="27"/>
+      <c r="D149" s="38"/>
+      <c r="E149" s="38"/>
+      <c r="F149" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G101" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="H101" s="23" t="s">
+      <c r="G149" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="H149" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="I101" s="11"/>
-      <c r="J101" s="11"/>
-    </row>
-    <row r="102" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B102" s="25"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="22" t="s">
+      <c r="I149" s="11"/>
+      <c r="J149" s="11"/>
+    </row>
+    <row r="150" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B150" s="27"/>
+      <c r="C150" s="27"/>
+      <c r="D150" s="38"/>
+      <c r="E150" s="38"/>
+      <c r="F150" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="G102" s="22" t="s">
+      <c r="G150" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="H102" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="I102" s="11"/>
-      <c r="J102" s="11"/>
-    </row>
-    <row r="103" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B103" s="25"/>
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="22" t="s">
+      <c r="H150" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="I150" s="11"/>
+      <c r="J150" s="11"/>
+    </row>
+    <row r="151" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B151" s="27"/>
+      <c r="C151" s="27"/>
+      <c r="D151" s="38"/>
+      <c r="E151" s="38"/>
+      <c r="F151" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G103" s="22" t="s">
+      <c r="G151" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="H103" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-    </row>
-    <row r="104" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B104" s="26">
+      <c r="H151" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="I151" s="11"/>
+      <c r="J151" s="11"/>
+    </row>
+    <row r="152" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B152" s="28">
         <v>2</v>
       </c>
-      <c r="C104" s="26">
-        <v>5</v>
-      </c>
-      <c r="D104" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="E104" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="F104" s="13" t="s">
+      <c r="C152" s="28">
+        <v>12</v>
+      </c>
+      <c r="D152" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="E152" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="F152" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="G104" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="H104" s="13"/>
-      <c r="I104" s="13"/>
-      <c r="J104" s="13"/>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B105" s="26"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="26"/>
-      <c r="E105" s="26"/>
-      <c r="F105" s="9" t="s">
+      <c r="G152" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="H152" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="I152" s="13"/>
+      <c r="J152" s="13"/>
+    </row>
+    <row r="153" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B153" s="28"/>
+      <c r="C153" s="28"/>
+      <c r="D153" s="41"/>
+      <c r="E153" s="41"/>
+      <c r="F153" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="G105" s="9" t="s">
+      <c r="G153" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="H105" s="9" t="s">
+      <c r="H153" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="I105" s="9"/>
-      <c r="J105" s="9"/>
-    </row>
-    <row r="106" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B106" s="26"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="26"/>
-      <c r="F106" s="33" t="s">
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
+    </row>
+    <row r="154" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B154" s="28"/>
+      <c r="C154" s="28"/>
+      <c r="D154" s="41"/>
+      <c r="E154" s="41"/>
+      <c r="F154" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="G106" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="H106" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="I106" s="9"/>
-      <c r="J106" s="9"/>
-    </row>
-    <row r="107" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B107" s="26"/>
-      <c r="C107" s="26"/>
-      <c r="D107" s="26"/>
-      <c r="E107" s="26"/>
-      <c r="F107" s="33" t="s">
+      <c r="G154" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="H154" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="I154" s="9"/>
+      <c r="J154" s="9"/>
+    </row>
+    <row r="155" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B155" s="28"/>
+      <c r="C155" s="28"/>
+      <c r="D155" s="41"/>
+      <c r="E155" s="41"/>
+      <c r="F155" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="G107" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="H107" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-    </row>
-    <row r="108" spans="2:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="26"/>
-      <c r="C108" s="26"/>
-      <c r="D108" s="26"/>
-      <c r="E108" s="26"/>
-      <c r="F108" s="33" t="s">
+      <c r="G155" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="H155" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="I155" s="9"/>
+      <c r="J155" s="9"/>
+    </row>
+    <row r="156" spans="2:10" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="28"/>
+      <c r="C156" s="28"/>
+      <c r="D156" s="41"/>
+      <c r="E156" s="41"/>
+      <c r="F156" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="G108" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H108" s="34" t="s">
+      <c r="G156" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="H156" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="I108" s="9"/>
-      <c r="J108" s="9"/>
-    </row>
-    <row r="109" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B109" s="26"/>
-      <c r="C109" s="26"/>
-      <c r="D109" s="26"/>
-      <c r="E109" s="26"/>
-      <c r="F109" s="33" t="s">
+      <c r="I156" s="9"/>
+      <c r="J156" s="9"/>
+    </row>
+    <row r="157" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B157" s="28"/>
+      <c r="C157" s="28"/>
+      <c r="D157" s="41"/>
+      <c r="E157" s="41"/>
+      <c r="F157" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="G109" s="33" t="s">
+      <c r="G157" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="H109" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="I109" s="9"/>
-      <c r="J109" s="9"/>
-    </row>
-    <row r="110" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B110" s="26"/>
-      <c r="C110" s="26"/>
-      <c r="D110" s="26"/>
-      <c r="E110" s="26"/>
-      <c r="F110" s="33" t="s">
+      <c r="H157" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="I157" s="9"/>
+      <c r="J157" s="9"/>
+    </row>
+    <row r="158" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B158" s="28"/>
+      <c r="C158" s="28"/>
+      <c r="D158" s="41"/>
+      <c r="E158" s="41"/>
+      <c r="F158" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="G110" s="33" t="s">
+      <c r="G158" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="H110" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="I110" s="9"/>
-      <c r="J110" s="9"/>
-    </row>
-    <row r="111" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B111" s="25">
+      <c r="H158" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I158" s="9"/>
+      <c r="J158" s="9"/>
+    </row>
+    <row r="159" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B159" s="27">
         <v>2</v>
       </c>
-      <c r="C111" s="25">
-        <v>6</v>
-      </c>
-      <c r="D111" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="E111" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="F111" s="20" t="s">
+      <c r="C159" s="27">
+        <v>13</v>
+      </c>
+      <c r="D159" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="E159" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="F159" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G111" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H111" s="20"/>
-      <c r="I111" s="20"/>
-      <c r="J111" s="20"/>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B112" s="25"/>
-      <c r="C112" s="25"/>
-      <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="11" t="s">
+      <c r="G159" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="H159" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="I159" s="20"/>
+      <c r="J159" s="20"/>
+    </row>
+    <row r="160" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B160" s="27"/>
+      <c r="C160" s="27"/>
+      <c r="D160" s="38"/>
+      <c r="E160" s="38"/>
+      <c r="F160" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="G112" s="11" t="s">
+      <c r="G160" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="H112" s="11" t="s">
+      <c r="H160" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="I112" s="11"/>
-      <c r="J112" s="11"/>
-    </row>
-    <row r="113" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B113" s="25"/>
-      <c r="C113" s="25"/>
-      <c r="D113" s="25"/>
-      <c r="E113" s="25"/>
-      <c r="F113" s="22" t="s">
+      <c r="I160" s="11"/>
+      <c r="J160" s="11"/>
+    </row>
+    <row r="161" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B161" s="27"/>
+      <c r="C161" s="27"/>
+      <c r="D161" s="38"/>
+      <c r="E161" s="38"/>
+      <c r="F161" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G113" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="H113" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="I113" s="11"/>
-      <c r="J113" s="11"/>
-    </row>
-    <row r="114" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B114" s="25"/>
-      <c r="C114" s="25"/>
-      <c r="D114" s="25"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="22" t="s">
+      <c r="G161" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H161" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="I161" s="11"/>
+      <c r="J161" s="11"/>
+    </row>
+    <row r="162" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B162" s="27"/>
+      <c r="C162" s="27"/>
+      <c r="D162" s="38"/>
+      <c r="E162" s="38"/>
+      <c r="F162" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="G114" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="H114" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="I114" s="11"/>
-      <c r="J114" s="11"/>
-    </row>
-    <row r="115" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="25"/>
-      <c r="C115" s="25"/>
-      <c r="D115" s="25"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="22" t="s">
+      <c r="G162" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="H162" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="I162" s="11"/>
+      <c r="J162" s="11"/>
+    </row>
+    <row r="163" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="27"/>
+      <c r="C163" s="27"/>
+      <c r="D163" s="38"/>
+      <c r="E163" s="38"/>
+      <c r="F163" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G115" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="H115" s="23" t="s">
+      <c r="G163" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="H163" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="I115" s="11"/>
-      <c r="J115" s="11"/>
-    </row>
-    <row r="116" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B116" s="25"/>
-      <c r="C116" s="25"/>
-      <c r="D116" s="25"/>
-      <c r="E116" s="25"/>
-      <c r="F116" s="22" t="s">
+      <c r="I163" s="11"/>
+      <c r="J163" s="11"/>
+    </row>
+    <row r="164" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B164" s="27"/>
+      <c r="C164" s="27"/>
+      <c r="D164" s="38"/>
+      <c r="E164" s="38"/>
+      <c r="F164" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="G116" s="22" t="s">
+      <c r="G164" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="H116" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="I116" s="11"/>
-      <c r="J116" s="11"/>
-    </row>
-    <row r="117" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B117" s="25"/>
-      <c r="C117" s="25"/>
-      <c r="D117" s="25"/>
-      <c r="E117" s="25"/>
-      <c r="F117" s="22" t="s">
+      <c r="H164" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="I164" s="11"/>
+      <c r="J164" s="11"/>
+    </row>
+    <row r="165" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B165" s="27"/>
+      <c r="C165" s="27"/>
+      <c r="D165" s="38"/>
+      <c r="E165" s="38"/>
+      <c r="F165" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G117" s="22" t="s">
+      <c r="G165" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="H117" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="I117" s="11"/>
-      <c r="J117" s="11"/>
-    </row>
-    <row r="118" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B118" s="26">
-        <v>2</v>
-      </c>
-      <c r="C118" s="26">
-        <v>7</v>
-      </c>
-      <c r="D118" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="E118" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="F118" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G118" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="13"/>
-    </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B119" s="26"/>
-      <c r="C119" s="26"/>
-      <c r="D119" s="26"/>
-      <c r="E119" s="26"/>
-      <c r="F119" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G119" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H119" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I119" s="9"/>
-      <c r="J119" s="9"/>
-    </row>
-    <row r="120" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B120" s="26"/>
-      <c r="C120" s="26"/>
-      <c r="D120" s="26"/>
-      <c r="E120" s="26"/>
-      <c r="F120" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G120" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="H120" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="I120" s="9"/>
-      <c r="J120" s="9"/>
-    </row>
-    <row r="121" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B121" s="26"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="26"/>
-      <c r="E121" s="26"/>
-      <c r="F121" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="G121" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="H121" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="I121" s="9"/>
-      <c r="J121" s="9"/>
-    </row>
-    <row r="122" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="26"/>
-      <c r="C122" s="26"/>
-      <c r="D122" s="26"/>
-      <c r="E122" s="26"/>
-      <c r="F122" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G122" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H122" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="I122" s="9"/>
-      <c r="J122" s="9"/>
-    </row>
-    <row r="123" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B123" s="26"/>
-      <c r="C123" s="26"/>
-      <c r="D123" s="26"/>
-      <c r="E123" s="26"/>
-      <c r="F123" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G123" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H123" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="I123" s="9"/>
-      <c r="J123" s="9"/>
-    </row>
-    <row r="124" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B124" s="26"/>
-      <c r="C124" s="26"/>
-      <c r="D124" s="26"/>
-      <c r="E124" s="26"/>
-      <c r="F124" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G124" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="H124" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="I124" s="9"/>
-      <c r="J124" s="9"/>
-    </row>
-    <row r="125" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B125" s="25">
-        <v>2</v>
-      </c>
-      <c r="C125" s="25">
-        <v>8</v>
-      </c>
-      <c r="D125" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="E125" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="F125" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G125" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="H125" s="38"/>
-      <c r="I125" s="20"/>
-      <c r="J125" s="20"/>
-    </row>
-    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B126" s="25"/>
-      <c r="C126" s="25"/>
-      <c r="D126" s="25"/>
-      <c r="E126" s="41"/>
-      <c r="F126" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="G126" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="H126" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="I126" s="11"/>
-      <c r="J126" s="11"/>
-    </row>
-    <row r="127" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B127" s="25"/>
-      <c r="C127" s="25"/>
-      <c r="D127" s="25"/>
-      <c r="E127" s="41"/>
-      <c r="F127" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="G127" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="H127" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="I127" s="11"/>
-      <c r="J127" s="11"/>
-    </row>
-    <row r="128" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B128" s="25"/>
-      <c r="C128" s="25"/>
-      <c r="D128" s="25"/>
-      <c r="E128" s="41"/>
-      <c r="F128" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="G128" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="H128" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="I128" s="11"/>
-      <c r="J128" s="11"/>
-    </row>
-    <row r="129" spans="2:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="25"/>
-      <c r="C129" s="25"/>
-      <c r="D129" s="25"/>
-      <c r="E129" s="41"/>
-      <c r="F129" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="G129" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="H129" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="I129" s="11"/>
-      <c r="J129" s="11"/>
-    </row>
-    <row r="130" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B130" s="25"/>
-      <c r="C130" s="25"/>
-      <c r="D130" s="25"/>
-      <c r="E130" s="41"/>
-      <c r="F130" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="G130" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="H130" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="I130" s="11"/>
-      <c r="J130" s="11"/>
-    </row>
-    <row r="131" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B131" s="25"/>
-      <c r="C131" s="25"/>
-      <c r="D131" s="25"/>
-      <c r="E131" s="41"/>
-      <c r="F131" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="G131" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="H131" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="I131" s="11"/>
-      <c r="J131" s="11"/>
-    </row>
-    <row r="132" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H165" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="I165" s="11"/>
+      <c r="J165" s="11"/>
+    </row>
+    <row r="166" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="177" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="178" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="179" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6098,23 +7061,58 @@
     <row r="494" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="495" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="496" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{B0953F3B-78FC-43F3-9402-DE0C5199EBA3}"/>
-  <mergeCells count="69">
-    <mergeCell ref="B125:B131"/>
-    <mergeCell ref="C125:C131"/>
-    <mergeCell ref="D125:D131"/>
-    <mergeCell ref="E125:E131"/>
-    <mergeCell ref="B118:B124"/>
-    <mergeCell ref="C118:C124"/>
-    <mergeCell ref="D118:D124"/>
-    <mergeCell ref="E118:E124"/>
-    <mergeCell ref="A2:A80"/>
-    <mergeCell ref="B104:B110"/>
-    <mergeCell ref="C104:C110"/>
-    <mergeCell ref="D104:D110"/>
-    <mergeCell ref="E104:E110"/>
+  <mergeCells count="89">
+    <mergeCell ref="B152:B158"/>
+    <mergeCell ref="C152:C158"/>
+    <mergeCell ref="D152:D158"/>
+    <mergeCell ref="E152:E158"/>
+    <mergeCell ref="B159:B165"/>
+    <mergeCell ref="C159:C165"/>
+    <mergeCell ref="D159:D165"/>
+    <mergeCell ref="E159:E165"/>
+    <mergeCell ref="B138:B144"/>
+    <mergeCell ref="C138:C144"/>
+    <mergeCell ref="D138:D144"/>
+    <mergeCell ref="E138:E144"/>
+    <mergeCell ref="B145:B151"/>
+    <mergeCell ref="C145:C151"/>
+    <mergeCell ref="D145:D151"/>
+    <mergeCell ref="E145:E151"/>
+    <mergeCell ref="B91:B96"/>
+    <mergeCell ref="C91:C96"/>
+    <mergeCell ref="D91:D96"/>
+    <mergeCell ref="E91:E96"/>
+    <mergeCell ref="B131:B137"/>
+    <mergeCell ref="C131:C137"/>
+    <mergeCell ref="D131:D137"/>
+    <mergeCell ref="E131:E137"/>
+    <mergeCell ref="B63:B71"/>
+    <mergeCell ref="C63:C71"/>
+    <mergeCell ref="D63:D71"/>
+    <mergeCell ref="E63:E71"/>
+    <mergeCell ref="B72:B80"/>
+    <mergeCell ref="C72:C80"/>
+    <mergeCell ref="D72:D80"/>
+    <mergeCell ref="E72:E80"/>
+    <mergeCell ref="B46:B54"/>
+    <mergeCell ref="C46:C54"/>
+    <mergeCell ref="D46:D54"/>
+    <mergeCell ref="E46:E54"/>
+    <mergeCell ref="B55:B62"/>
+    <mergeCell ref="C55:C62"/>
+    <mergeCell ref="D55:D62"/>
+    <mergeCell ref="E55:E62"/>
+    <mergeCell ref="B10:B18"/>
+    <mergeCell ref="E28:E36"/>
+    <mergeCell ref="B37:B45"/>
+    <mergeCell ref="C37:C45"/>
+    <mergeCell ref="D37:D45"/>
+    <mergeCell ref="E37:E45"/>
+    <mergeCell ref="B28:B36"/>
+    <mergeCell ref="C28:C36"/>
+    <mergeCell ref="D28:D36"/>
     <mergeCell ref="B111:B117"/>
     <mergeCell ref="C111:C117"/>
     <mergeCell ref="D111:D117"/>
@@ -6123,6 +7121,19 @@
     <mergeCell ref="C81:C84"/>
     <mergeCell ref="D81:D84"/>
     <mergeCell ref="E81:E84"/>
+    <mergeCell ref="B97:B103"/>
+    <mergeCell ref="C97:C103"/>
+    <mergeCell ref="D97:D103"/>
+    <mergeCell ref="E97:E103"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="C85:C90"/>
+    <mergeCell ref="D85:D90"/>
+    <mergeCell ref="E85:E90"/>
+    <mergeCell ref="A2:A80"/>
+    <mergeCell ref="B104:B110"/>
+    <mergeCell ref="C104:C110"/>
+    <mergeCell ref="D104:D110"/>
+    <mergeCell ref="E104:E110"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="C2:C9"/>
     <mergeCell ref="D2:D9"/>
@@ -6134,43 +7145,14 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="D10:D18"/>
     <mergeCell ref="C10:C18"/>
-    <mergeCell ref="B10:B18"/>
-    <mergeCell ref="E28:E36"/>
-    <mergeCell ref="B37:B45"/>
-    <mergeCell ref="C37:C45"/>
-    <mergeCell ref="D37:D45"/>
-    <mergeCell ref="E37:E45"/>
-    <mergeCell ref="B28:B36"/>
-    <mergeCell ref="C28:C36"/>
-    <mergeCell ref="D28:D36"/>
-    <mergeCell ref="B46:B54"/>
-    <mergeCell ref="C46:C54"/>
-    <mergeCell ref="D46:D54"/>
-    <mergeCell ref="E46:E54"/>
-    <mergeCell ref="B55:B62"/>
-    <mergeCell ref="C55:C62"/>
-    <mergeCell ref="D55:D62"/>
-    <mergeCell ref="E55:E62"/>
-    <mergeCell ref="B63:B71"/>
-    <mergeCell ref="C63:C71"/>
-    <mergeCell ref="D63:D71"/>
-    <mergeCell ref="E63:E71"/>
-    <mergeCell ref="B72:B80"/>
-    <mergeCell ref="C72:C80"/>
-    <mergeCell ref="D72:D80"/>
-    <mergeCell ref="E72:E80"/>
-    <mergeCell ref="B97:B103"/>
-    <mergeCell ref="C97:C103"/>
-    <mergeCell ref="D97:D103"/>
-    <mergeCell ref="E97:E103"/>
-    <mergeCell ref="B85:B90"/>
-    <mergeCell ref="C85:C90"/>
-    <mergeCell ref="D85:D90"/>
-    <mergeCell ref="E85:E90"/>
-    <mergeCell ref="B91:B96"/>
-    <mergeCell ref="C91:C96"/>
-    <mergeCell ref="D91:D96"/>
-    <mergeCell ref="E91:E96"/>
+    <mergeCell ref="B125:B130"/>
+    <mergeCell ref="C125:C130"/>
+    <mergeCell ref="D125:D130"/>
+    <mergeCell ref="E125:E130"/>
+    <mergeCell ref="B118:B124"/>
+    <mergeCell ref="C118:C124"/>
+    <mergeCell ref="D118:D124"/>
+    <mergeCell ref="E118:E124"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6179,10 +7161,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B204A399-C202-4A7B-9C11-B42BFE1631E2}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A25" sqref="A25:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6196,13 +7178,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -6358,13 +7340,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
+      <c r="A11" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
@@ -6452,13 +7434,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
+      <c r="A17" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
@@ -6545,11 +7527,89 @@
         <v>101</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>6</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="19">
+        <v>45301</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
+        <v>7</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="18">
+        <v>127.35</v>
+      </c>
+      <c r="D26" s="19">
+        <v>45304</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>8</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="18">
+        <v>50</v>
+      </c>
+      <c r="D27" s="19">
+        <v>45305</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>